<commit_message>
some remarks were made and mistakes were fixed
</commit_message>
<xml_diff>
--- a/bug_report_example.xlsx
+++ b/bug_report_example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -65,6 +65,46 @@
   </si>
   <si>
     <t>Major</t>
+  </si>
+  <si>
+    <t>1. Open the Coursera home page https://www.coursera.org and select My courses in the user's Profile menu</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1HhQPO1SFyOq9GkpbIMk8PyxrwsexQIwR/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13HycClCRQhx2ugWchpoez6d22INofK7r/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1KYHwQk9cy2qLulLyU-R7VrBwkAGhyxZn/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Attachments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploads error page (see "error_page_uploads.jpg"), in the browsers console appears error "TypeError: Cannot read property 'match' of undefined" (see the log file "www.coursera.org-error.log"). </t>
+  </si>
+  <si>
+    <t>[Desktop] Error page uploads after trying to open a discussion "Can't submit a file in the "Hello, %username!" for the task "Programming Assignment: Hello, %username!"</t>
+  </si>
+  <si>
+    <t>The discussion page "Can't submit a file in the "Hello, %username!" for the task "Programming Assignment: Hello, %username!" uploads in the modal window above the task page where a user can read a topic, discussion, leave comments and likes</t>
+  </si>
+  <si>
+    <t>The problem was analyzed and it was discovered, if the user's account who has created the discussion was deleted/freezed (including users who logged with a social media login) this defect appears. This problem is actual for any topic where the user's account was deleted/freezed. See the log file "www.coursera.org-error.log" for more details</t>
+  </si>
+  <si>
+    <t>2. Find the course "Основы програмирования на Python" in the user's Current courses and press on the button Go To Course</t>
+  </si>
+  <si>
+    <t>3. In the side Navigation menu select Week 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. In main section select the task "Programming Assignment: Hello, %username!"
+</t>
+  </si>
+  <si>
+    <t>5. In the side Discussion menu select the topic "Can't submit a file in the "Hello, %username!" (see "discussion_cant_submit_file.png")</t>
   </si>
   <si>
     <r>
@@ -109,7 +149,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> PROD (user-agent: Windows 10, Chrome version 90.0.4430.85). </t>
+      <t xml:space="preserve"> PROD (user-agent: Windows 10, Chrome version 90.0.4430.85). Open browser's DevTools to see more details about the defect. </t>
     </r>
     <r>
       <rPr>
@@ -134,60 +174,25 @@
       <t xml:space="preserve"> on the Overview course page (https://www.coursera.org/learn/python-osnovy-programmirovaniya/home/welcome) in the side Navigation select "Discussion Forums" =&gt; "Week 1" =&gt; "Can't submit a file in the "Hello, %username!"</t>
     </r>
   </si>
-  <si>
-    <t>1. Open the Coursera home page https://www.coursera.org and select My courses in the user's Profile menu</t>
-  </si>
-  <si>
-    <t>2. Press f12 to open Chrome Dev tools and go to console tab</t>
-  </si>
-  <si>
-    <t>3. Find the course "Основы програмирования на Python" in the user's Current courses and press on the button Go To Course</t>
-  </si>
-  <si>
-    <t>4. In the side Navigation menu select Week 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. In main section select the task "Programming Assignment: Hello, %username!"
-</t>
-  </si>
-  <si>
-    <t>6. In the side Discussion menu select the topic "Can't submit a file in the "Hello, %username!" (see "discussion_cant_submit_file.png")</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1HhQPO1SFyOq9GkpbIMk8PyxrwsexQIwR/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/13HycClCRQhx2ugWchpoez6d22INofK7r/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1KYHwQk9cy2qLulLyU-R7VrBwkAGhyxZn/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Attachments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uploads error page (see "error_page_uploads.jpg"), in the browsers console appears error "TypeError: Cannot read property 'match' of undefined" (see the log file "www.coursera.org-error.log"). </t>
-  </si>
-  <si>
-    <t>[Desktop] Error page uploads after trying to open a discussion "Can't submit a file in the "Hello, %username!" for the task "Programming Assignment: Hello, %username!"</t>
-  </si>
-  <si>
-    <t>The discussion page "Can't submit a file in the "Hello, %username!" for the task "Programming Assignment: Hello, %username!" uploads in the modal window above the task page where a user can read a topic, discussion, leave comments and likes</t>
-  </si>
-  <si>
-    <t>The problem was analyzed and it was discovered, if the user's account who has created the discussion was deleted/freezed (including users who logged with a social media login) this defect appears. This problem is actual for any topic where the user's account was deleted/freezed. See the log file "www.coursera.org-error.log" for more details</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -300,13 +305,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -316,22 +330,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -639,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N9"/>
+  <dimension ref="B3:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N9"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,194 +669,177 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="M3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="2:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="4"/>
+      <c r="N8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I4:I9"/>
-    <mergeCell ref="J4:J9"/>
-    <mergeCell ref="K4:K9"/>
-    <mergeCell ref="L4:L9"/>
-    <mergeCell ref="N4:N9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="D4:D9"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="G4:G9"/>
-    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="H4:H8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="I4:I8"/>
+    <mergeCell ref="J4:J8"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="L4:L8"/>
+    <mergeCell ref="N4:N8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1"/>
-    <hyperlink ref="M8" r:id="rId2"/>
-    <hyperlink ref="M9" r:id="rId3"/>
+    <hyperlink ref="M6" r:id="rId1"/>
+    <hyperlink ref="M7" r:id="rId2"/>
+    <hyperlink ref="M8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>